<commit_message>
CDFs implemented. Model working. SDVs set to values believed to work.
</commit_message>
<xml_diff>
--- a/cost_model/cost_model.xlsx
+++ b/cost_model/cost_model.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\knech\OneDrive\Documents\ASE6002\ModelProject\cost_model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E36C5540-164E-4118-89D6-ACC5F318F909}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B419944E-7C9D-4821-9DB0-661A8B92BD60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="3" xr2:uid="{0BE88EB2-3A1E-BD41-82F4-6438F84B674A}"/>
   </bookViews>
@@ -735,7 +735,7 @@
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="16">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -6465,7 +6465,7 @@
       <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.46484375" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="11.46484375" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="31.6640625" style="25" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.33203125" style="25" customWidth="1"/>
@@ -6479,7 +6479,7 @@
     <col min="258" max="16384" width="11.46484375" style="25"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B1" s="25" t="s">
         <v>0</v>
       </c>
@@ -6487,13 +6487,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="F2" s="25" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="13.15" thickBot="1"/>
-    <row r="5" spans="1:9" ht="13.5" thickBot="1">
+    <row r="4" spans="1:9" ht="13.15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="5" spans="1:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A5" s="26" t="s">
         <v>3</v>
       </c>
@@ -6502,7 +6502,7 @@
       </c>
       <c r="D5" s="28"/>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="29" t="s">
         <v>5</v>
       </c>
@@ -6510,7 +6510,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="31" t="s">
         <v>6</v>
       </c>
@@ -6519,7 +6519,7 @@
       </c>
       <c r="D7" s="28"/>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="31" t="s">
         <v>7</v>
       </c>
@@ -6528,13 +6528,13 @@
         <v>159</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="13.15" thickBot="1">
+    <row r="9" spans="1:9" ht="13.15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="33" t="s">
         <v>8</v>
       </c>
       <c r="B9" s="32"/>
     </row>
-    <row r="10" spans="1:9" ht="13.5" thickBot="1">
+    <row r="10" spans="1:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A10" s="31" t="s">
         <v>9</v>
       </c>
@@ -6551,7 +6551,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" s="33" t="s">
         <v>10</v>
       </c>
@@ -6570,7 +6570,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" s="31" t="s">
         <v>11</v>
       </c>
@@ -6586,7 +6586,7 @@
         <v>307500</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" s="31" t="s">
         <v>12</v>
       </c>
@@ -6604,7 +6604,7 @@
         <v>1601600</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="13.15" thickBot="1">
+    <row r="14" spans="1:9" ht="13.15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="31" t="s">
         <v>13</v>
       </c>
@@ -6622,7 +6622,7 @@
         <v>1.04</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="13.5" thickBot="1">
+    <row r="15" spans="1:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A15" s="31" t="s">
         <v>14</v>
       </c>
@@ -6641,13 +6641,13 @@
         <v>3199100</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="13.15" thickBot="1">
+    <row r="16" spans="1:9" ht="13.15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" s="31" t="s">
         <v>15</v>
       </c>
       <c r="B16" s="32"/>
     </row>
-    <row r="17" spans="1:8" ht="13.5" thickBot="1">
+    <row r="17" spans="1:8" ht="13.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A17" s="31" t="s">
         <v>16</v>
       </c>
@@ -6661,7 +6661,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" s="31" t="s">
         <v>17</v>
       </c>
@@ -6673,7 +6673,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" s="46" t="s">
         <v>18</v>
       </c>
@@ -6694,7 +6694,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" s="46" t="s">
         <v>19</v>
       </c>
@@ -6712,7 +6712,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" s="46" t="s">
         <v>20</v>
       </c>
@@ -6726,7 +6726,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="13.15" thickBot="1">
+    <row r="22" spans="1:8" ht="13.15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" s="46" t="s">
         <v>21</v>
       </c>
@@ -6738,7 +6738,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="13.5" thickBot="1">
+    <row r="23" spans="1:8" ht="13.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A23" s="33" t="s">
         <v>22</v>
       </c>
@@ -6747,7 +6747,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A24" s="33" t="s">
         <v>23</v>
       </c>
@@ -6756,7 +6756,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A25" s="31" t="s">
         <v>24</v>
       </c>
@@ -6765,7 +6765,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A26" s="31" t="s">
         <v>25</v>
       </c>
@@ -6774,7 +6774,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="13.15" thickBot="1">
+    <row r="27" spans="1:8" ht="13.15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A27" s="31" t="s">
         <v>26</v>
       </c>
@@ -6783,13 +6783,13 @@
         <v>179</v>
       </c>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A28" s="33" t="s">
         <v>27</v>
       </c>
       <c r="B28" s="32"/>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A29" s="31" t="s">
         <v>28</v>
       </c>
@@ -6797,7 +6797,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A30" s="31" t="s">
         <v>29</v>
       </c>
@@ -6805,7 +6805,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A31" s="38" t="s">
         <v>30</v>
       </c>
@@ -6817,7 +6817,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A32" s="39" t="s">
         <v>31</v>
       </c>
@@ -6826,7 +6826,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="33" spans="1:9" ht="13.15" thickBot="1">
+    <row r="33" spans="1:9" ht="13.15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A33" s="40" t="s">
         <v>32</v>
       </c>
@@ -6835,7 +6835,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="34" spans="1:9">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B34" s="25">
         <f>SUM(B6:B33)</f>
         <v>293</v>
@@ -6845,7 +6845,7 @@
         <v>5160</v>
       </c>
     </row>
-    <row r="35" spans="1:9">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
       <c r="F35" s="25">
         <f>75+142+400</f>
         <v>617</v>
@@ -6855,7 +6855,7 @@
         <v>4.47</v>
       </c>
     </row>
-    <row r="36" spans="1:9">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
       <c r="F36" s="47">
         <f>F35/6</f>
         <v>102.83333333333333</v>
@@ -6872,18 +6872,18 @@
         <v>18625</v>
       </c>
     </row>
-    <row r="37" spans="1:9">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
       <c r="G37" s="53">
         <f>G36*12</f>
         <v>8.94</v>
       </c>
     </row>
-    <row r="44" spans="1:9">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
       <c r="G44" s="25" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="45" spans="1:9">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
       <c r="G45" s="25" t="s">
         <v>182</v>
       </c>
@@ -6911,9 +6911,9 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.3984375" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="11.3984375" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:23" ht="14.25">
+    <row r="1" spans="1:23" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A1" s="15"/>
       <c r="B1" s="15" t="s">
         <v>1</v>
@@ -6972,7 +6972,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:23" ht="14.25">
+    <row r="2" spans="1:23" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A2" s="12" t="s">
         <v>50</v>
       </c>
@@ -7043,7 +7043,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:23" ht="14.25">
+    <row r="3" spans="1:23" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A3" s="12"/>
       <c r="B3" s="12"/>
       <c r="C3" s="12"/>
@@ -7102,7 +7102,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="4" spans="1:23">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.35">
       <c r="J4" s="13"/>
       <c r="K4" s="13" t="s">
         <v>60</v>
@@ -7146,7 +7146,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="5" spans="1:23">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A5" s="2"/>
       <c r="K5" t="s">
         <v>62</v>
@@ -7190,7 +7190,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="6" spans="1:23">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A6" s="2"/>
       <c r="K6" t="s">
         <v>63</v>
@@ -7234,7 +7234,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="7" spans="1:23">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.35">
       <c r="K7" t="s">
         <v>64</v>
       </c>
@@ -7277,7 +7277,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="8" spans="1:23">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.35">
       <c r="K8" t="s">
         <v>65</v>
       </c>
@@ -7320,7 +7320,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="9" spans="1:23">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.35">
       <c r="K9" t="s">
         <v>66</v>
       </c>
@@ -7363,7 +7363,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="10" spans="1:23">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.35">
       <c r="K10" t="s">
         <v>67</v>
       </c>
@@ -7406,7 +7406,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="11" spans="1:23">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.35">
       <c r="K11" t="s">
         <v>68</v>
       </c>
@@ -7449,7 +7449,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="12" spans="1:23">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.35">
       <c r="K12" t="s">
         <v>69</v>
       </c>
@@ -7492,7 +7492,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="13" spans="1:23">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.35">
       <c r="K13" t="s">
         <v>70</v>
       </c>
@@ -7535,7 +7535,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="14" spans="1:23">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.35">
       <c r="K14" t="s">
         <v>71</v>
       </c>
@@ -7578,7 +7578,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="15" spans="1:23">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.35">
       <c r="K15" t="s">
         <v>72</v>
       </c>
@@ -7621,7 +7621,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="16" spans="1:23">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.35">
       <c r="K16" t="s">
         <v>73</v>
       </c>
@@ -7664,7 +7664,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="17" spans="11:23">
+    <row r="17" spans="11:23" x14ac:dyDescent="0.35">
       <c r="K17" t="s">
         <v>74</v>
       </c>
@@ -7707,7 +7707,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="18" spans="11:23">
+    <row r="18" spans="11:23" x14ac:dyDescent="0.35">
       <c r="K18" t="s">
         <v>75</v>
       </c>
@@ -7750,7 +7750,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="19" spans="11:23">
+    <row r="19" spans="11:23" x14ac:dyDescent="0.35">
       <c r="K19" t="s">
         <v>76</v>
       </c>
@@ -7793,7 +7793,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="20" spans="11:23">
+    <row r="20" spans="11:23" x14ac:dyDescent="0.35">
       <c r="K20" t="s">
         <v>77</v>
       </c>
@@ -7836,7 +7836,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="21" spans="11:23">
+    <row r="21" spans="11:23" x14ac:dyDescent="0.35">
       <c r="K21" t="s">
         <v>78</v>
       </c>
@@ -7879,7 +7879,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="22" spans="11:23">
+    <row r="22" spans="11:23" x14ac:dyDescent="0.35">
       <c r="K22" t="s">
         <v>79</v>
       </c>
@@ -7922,7 +7922,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="23" spans="11:23">
+    <row r="23" spans="11:23" x14ac:dyDescent="0.35">
       <c r="K23" t="s">
         <v>80</v>
       </c>
@@ -7965,7 +7965,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="24" spans="11:23">
+    <row r="24" spans="11:23" x14ac:dyDescent="0.35">
       <c r="K24" t="s">
         <v>81</v>
       </c>
@@ -8008,7 +8008,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="25" spans="11:23">
+    <row r="25" spans="11:23" x14ac:dyDescent="0.35">
       <c r="K25" t="s">
         <v>82</v>
       </c>
@@ -8051,7 +8051,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="26" spans="11:23">
+    <row r="26" spans="11:23" x14ac:dyDescent="0.35">
       <c r="K26" t="s">
         <v>83</v>
       </c>
@@ -8094,7 +8094,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="27" spans="11:23">
+    <row r="27" spans="11:23" x14ac:dyDescent="0.35">
       <c r="K27" t="s">
         <v>84</v>
       </c>
@@ -8137,7 +8137,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="28" spans="11:23">
+    <row r="28" spans="11:23" x14ac:dyDescent="0.35">
       <c r="K28" t="s">
         <v>85</v>
       </c>
@@ -8180,7 +8180,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="29" spans="11:23">
+    <row r="29" spans="11:23" x14ac:dyDescent="0.35">
       <c r="K29" t="s">
         <v>86</v>
       </c>
@@ -8223,7 +8223,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="30" spans="11:23">
+    <row r="30" spans="11:23" x14ac:dyDescent="0.35">
       <c r="K30" t="s">
         <v>87</v>
       </c>
@@ -8266,7 +8266,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="31" spans="11:23">
+    <row r="31" spans="11:23" x14ac:dyDescent="0.35">
       <c r="K31" t="s">
         <v>88</v>
       </c>
@@ -8309,7 +8309,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="32" spans="11:23">
+    <row r="32" spans="11:23" x14ac:dyDescent="0.35">
       <c r="K32" t="s">
         <v>89</v>
       </c>
@@ -8352,7 +8352,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="33" spans="10:23">
+    <row r="33" spans="10:23" x14ac:dyDescent="0.35">
       <c r="K33" t="s">
         <v>90</v>
       </c>
@@ -8395,7 +8395,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="34" spans="10:23">
+    <row r="34" spans="10:23" x14ac:dyDescent="0.35">
       <c r="K34" t="s">
         <v>91</v>
       </c>
@@ -8438,7 +8438,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="35" spans="10:23">
+    <row r="35" spans="10:23" x14ac:dyDescent="0.35">
       <c r="J35" s="13"/>
       <c r="K35" s="13" t="s">
         <v>92</v>
@@ -8482,7 +8482,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="36" spans="10:23">
+    <row r="36" spans="10:23" x14ac:dyDescent="0.35">
       <c r="J36" s="13"/>
       <c r="K36" s="13" t="s">
         <v>93</v>
@@ -8526,7 +8526,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="37" spans="10:23">
+    <row r="37" spans="10:23" x14ac:dyDescent="0.35">
       <c r="J37" s="13"/>
       <c r="K37" s="13" t="s">
         <v>94</v>
@@ -8570,7 +8570,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="38" spans="10:23">
+    <row r="38" spans="10:23" x14ac:dyDescent="0.35">
       <c r="J38" s="13"/>
       <c r="K38" s="13" t="s">
         <v>95</v>
@@ -8614,7 +8614,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="39" spans="10:23">
+    <row r="39" spans="10:23" x14ac:dyDescent="0.35">
       <c r="J39" s="13"/>
       <c r="K39" s="13" t="s">
         <v>96</v>
@@ -8658,7 +8658,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="40" spans="10:23">
+    <row r="40" spans="10:23" x14ac:dyDescent="0.35">
       <c r="J40" s="13"/>
       <c r="K40" s="13" t="s">
         <v>97</v>
@@ -8702,7 +8702,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="41" spans="10:23">
+    <row r="41" spans="10:23" x14ac:dyDescent="0.35">
       <c r="J41" s="13"/>
       <c r="K41" s="13" t="s">
         <v>98</v>
@@ -8746,7 +8746,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="42" spans="10:23">
+    <row r="42" spans="10:23" x14ac:dyDescent="0.35">
       <c r="J42" s="13"/>
       <c r="K42" s="13" t="s">
         <v>99</v>
@@ -8790,7 +8790,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="43" spans="10:23">
+    <row r="43" spans="10:23" x14ac:dyDescent="0.35">
       <c r="J43" s="13"/>
       <c r="K43" s="13" t="s">
         <v>100</v>
@@ -8834,7 +8834,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="44" spans="10:23">
+    <row r="44" spans="10:23" x14ac:dyDescent="0.35">
       <c r="J44" s="13"/>
       <c r="K44" s="13" t="s">
         <v>101</v>
@@ -8878,7 +8878,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="45" spans="10:23">
+    <row r="45" spans="10:23" x14ac:dyDescent="0.35">
       <c r="J45" s="13"/>
       <c r="K45" s="13" t="s">
         <v>102</v>
@@ -8922,7 +8922,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="46" spans="10:23">
+    <row r="46" spans="10:23" x14ac:dyDescent="0.35">
       <c r="J46" s="13"/>
       <c r="K46" s="13" t="s">
         <v>103</v>
@@ -8966,7 +8966,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="47" spans="10:23">
+    <row r="47" spans="10:23" x14ac:dyDescent="0.35">
       <c r="J47" s="13"/>
       <c r="K47" s="13" t="s">
         <v>104</v>
@@ -9010,7 +9010,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="48" spans="10:23">
+    <row r="48" spans="10:23" x14ac:dyDescent="0.35">
       <c r="J48" s="13"/>
       <c r="K48" s="13" t="s">
         <v>105</v>
@@ -9054,7 +9054,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="49" spans="10:23">
+    <row r="49" spans="10:23" x14ac:dyDescent="0.35">
       <c r="J49" s="13"/>
       <c r="K49" s="13" t="s">
         <v>106</v>
@@ -9098,7 +9098,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="50" spans="10:23">
+    <row r="50" spans="10:23" x14ac:dyDescent="0.35">
       <c r="K50" t="s">
         <v>107</v>
       </c>
@@ -9141,7 +9141,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="51" spans="10:23">
+    <row r="51" spans="10:23" x14ac:dyDescent="0.35">
       <c r="K51" t="s">
         <v>108</v>
       </c>
@@ -9184,7 +9184,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="52" spans="10:23">
+    <row r="52" spans="10:23" x14ac:dyDescent="0.35">
       <c r="K52" t="s">
         <v>109</v>
       </c>
@@ -9227,7 +9227,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="53" spans="10:23">
+    <row r="53" spans="10:23" x14ac:dyDescent="0.35">
       <c r="K53" t="s">
         <v>110</v>
       </c>
@@ -9270,7 +9270,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="54" spans="10:23">
+    <row r="54" spans="10:23" x14ac:dyDescent="0.35">
       <c r="K54" t="s">
         <v>111</v>
       </c>
@@ -9313,7 +9313,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="55" spans="10:23">
+    <row r="55" spans="10:23" x14ac:dyDescent="0.35">
       <c r="K55" t="s">
         <v>112</v>
       </c>
@@ -9356,7 +9356,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="56" spans="10:23">
+    <row r="56" spans="10:23" x14ac:dyDescent="0.35">
       <c r="K56" t="s">
         <v>113</v>
       </c>
@@ -9399,7 +9399,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="57" spans="10:23">
+    <row r="57" spans="10:23" x14ac:dyDescent="0.35">
       <c r="K57" t="s">
         <v>114</v>
       </c>
@@ -9442,7 +9442,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="58" spans="10:23">
+    <row r="58" spans="10:23" x14ac:dyDescent="0.35">
       <c r="K58" t="s">
         <v>115</v>
       </c>
@@ -9485,7 +9485,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="59" spans="10:23">
+    <row r="59" spans="10:23" x14ac:dyDescent="0.35">
       <c r="K59" t="s">
         <v>116</v>
       </c>
@@ -9528,7 +9528,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="60" spans="10:23">
+    <row r="60" spans="10:23" x14ac:dyDescent="0.35">
       <c r="K60" t="s">
         <v>117</v>
       </c>
@@ -9571,7 +9571,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="61" spans="10:23">
+    <row r="61" spans="10:23" x14ac:dyDescent="0.35">
       <c r="K61" t="s">
         <v>118</v>
       </c>
@@ -9629,14 +9629,14 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="9" max="9" width="16.265625" customWidth="1"/>
     <col min="12" max="12" width="28" customWidth="1"/>
     <col min="15" max="15" width="8.73046875" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>1</v>
       </c>
@@ -9647,7 +9647,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="2" spans="1:19" ht="13.15" thickBot="1">
+    <row r="2" spans="1:19" ht="13.15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>120</v>
       </c>
@@ -9686,7 +9686,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="13.15" thickBot="1">
+    <row r="3" spans="1:19" ht="13.15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D3" t="s">
         <v>52</v>
       </c>
@@ -9724,7 +9724,7 @@
         <v>0.66849999999999987</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="13.15" thickBot="1">
+    <row r="4" spans="1:19" ht="13.15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="I4" s="4">
         <v>30</v>
       </c>
@@ -9752,7 +9752,7 @@
         <v>0.52899999999999991</v>
       </c>
     </row>
-    <row r="5" spans="1:19" ht="13.15" thickBot="1">
+    <row r="5" spans="1:19" ht="13.15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="I5" s="4">
         <v>30</v>
       </c>
@@ -9780,7 +9780,7 @@
         <v>0.25099999999999989</v>
       </c>
     </row>
-    <row r="6" spans="1:19" ht="13.15" thickBot="1">
+    <row r="6" spans="1:19" ht="13.15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="I6" s="4">
         <v>30</v>
       </c>
@@ -9808,7 +9808,7 @@
         <v>0.40300000000000002</v>
       </c>
     </row>
-    <row r="7" spans="1:19" ht="13.15" thickBot="1">
+    <row r="7" spans="1:19" ht="13.15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="I7" s="4">
         <v>30</v>
       </c>
@@ -9836,7 +9836,7 @@
         <v>1.113</v>
       </c>
     </row>
-    <row r="8" spans="1:19" ht="13.15" thickBot="1">
+    <row r="8" spans="1:19" ht="13.15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="I8" s="4">
         <v>35</v>
       </c>
@@ -9864,7 +9864,7 @@
         <v>0.6551428571428568</v>
       </c>
     </row>
-    <row r="9" spans="1:19" ht="13.15" thickBot="1">
+    <row r="9" spans="1:19" ht="13.15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="I9" s="4">
         <v>35</v>
       </c>
@@ -9892,7 +9892,7 @@
         <v>0.34357142857142842</v>
       </c>
     </row>
-    <row r="10" spans="1:19" ht="13.15" thickBot="1">
+    <row r="10" spans="1:19" ht="13.15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="I10" s="4">
         <v>35</v>
       </c>
@@ -9920,7 +9920,7 @@
         <v>0.31099999999999994</v>
       </c>
     </row>
-    <row r="11" spans="1:19" ht="13.15" thickBot="1">
+    <row r="11" spans="1:19" ht="13.15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="I11" s="4">
         <v>35</v>
       </c>
@@ -9948,7 +9948,7 @@
         <v>0.28571428571428559</v>
       </c>
     </row>
-    <row r="12" spans="1:19" ht="13.15" thickBot="1">
+    <row r="12" spans="1:19" ht="13.15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="I12" s="4">
         <v>35</v>
       </c>
@@ -9976,7 +9976,7 @@
         <v>0.81114285714285694</v>
       </c>
     </row>
-    <row r="13" spans="1:19" ht="13.15" thickBot="1">
+    <row r="13" spans="1:19" ht="13.15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="I13" s="4">
         <v>40</v>
       </c>
@@ -10004,7 +10004,7 @@
         <v>0.22512500000000024</v>
       </c>
     </row>
-    <row r="14" spans="1:19" ht="13.15" thickBot="1">
+    <row r="14" spans="1:19" ht="13.15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="I14" s="4">
         <v>40</v>
       </c>
@@ -10032,7 +10032,7 @@
         <v>0.54387500000000011</v>
       </c>
     </row>
-    <row r="15" spans="1:19" ht="13.5" thickBot="1">
+    <row r="15" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="I15" s="4">
         <v>40</v>
       </c>
@@ -10063,7 +10063,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="16" spans="1:19" ht="13.15" thickBot="1">
+    <row r="16" spans="1:19" ht="13.15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="I16" s="4">
         <v>40</v>
       </c>
@@ -10091,7 +10091,7 @@
         <v>0.26337500000000014</v>
       </c>
     </row>
-    <row r="17" spans="9:24" ht="13.5" thickBot="1">
+    <row r="17" spans="9:24" ht="13.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="I17" s="4">
         <v>45</v>
       </c>
@@ -10122,7 +10122,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="18" spans="9:24" ht="13.15" thickBot="1">
+    <row r="18" spans="9:24" ht="13.15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="I18" s="4">
         <v>45</v>
       </c>
@@ -10150,7 +10150,7 @@
         <v>0.43366666666666664</v>
       </c>
     </row>
-    <row r="19" spans="9:24" ht="13.5" thickBot="1">
+    <row r="19" spans="9:24" ht="13.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="I19" s="4">
         <v>45</v>
       </c>
@@ -10181,7 +10181,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="20" spans="9:24" ht="13.15" thickBot="1">
+    <row r="20" spans="9:24" ht="13.15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="I20" s="4">
         <v>45</v>
       </c>
@@ -10209,7 +10209,7 @@
         <v>0.68233333333333324</v>
       </c>
     </row>
-    <row r="21" spans="9:24" ht="13.15" thickBot="1">
+    <row r="21" spans="9:24" ht="13.15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="I21" s="4">
         <v>45</v>
       </c>
@@ -10252,7 +10252,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="22" spans="9:24">
+    <row r="22" spans="9:24" x14ac:dyDescent="0.35">
       <c r="I22" s="4">
         <v>45</v>
       </c>
@@ -10280,7 +10280,7 @@
         <v>0.8616666666666668</v>
       </c>
     </row>
-    <row r="23" spans="9:24">
+    <row r="23" spans="9:24" x14ac:dyDescent="0.35">
       <c r="I23" s="6">
         <v>40</v>
       </c>
@@ -10299,7 +10299,7 @@
         <v>1.4746250000000001</v>
       </c>
     </row>
-    <row r="24" spans="9:24">
+    <row r="24" spans="9:24" x14ac:dyDescent="0.35">
       <c r="I24" s="6">
         <v>45</v>
       </c>
@@ -10330,7 +10330,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="25" spans="9:24">
+    <row r="25" spans="9:24" x14ac:dyDescent="0.35">
       <c r="I25" s="6">
         <v>35</v>
       </c>
@@ -10346,7 +10346,7 @@
         <v>0.49999999999999978</v>
       </c>
     </row>
-    <row r="26" spans="9:24">
+    <row r="26" spans="9:24" x14ac:dyDescent="0.35">
       <c r="I26" s="6">
         <v>45</v>
       </c>
@@ -10365,7 +10365,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="27" spans="9:24">
+    <row r="27" spans="9:24" x14ac:dyDescent="0.35">
       <c r="I27" s="6">
         <v>50</v>
       </c>
@@ -10387,7 +10387,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="28" spans="9:24">
+    <row r="28" spans="9:24" x14ac:dyDescent="0.35">
       <c r="I28" s="6">
         <v>45</v>
       </c>
@@ -10403,7 +10403,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="9:24">
+    <row r="29" spans="9:24" x14ac:dyDescent="0.35">
       <c r="I29" s="6">
         <v>45</v>
       </c>
@@ -10422,7 +10422,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="30" spans="9:24">
+    <row r="30" spans="9:24" x14ac:dyDescent="0.35">
       <c r="I30" s="6">
         <v>40</v>
       </c>
@@ -10438,7 +10438,7 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="31" spans="9:24">
+    <row r="31" spans="9:24" x14ac:dyDescent="0.35">
       <c r="I31" s="6">
         <v>50</v>
       </c>
@@ -10454,7 +10454,7 @@
         <v>1.0999999999999996</v>
       </c>
     </row>
-    <row r="32" spans="9:24">
+    <row r="32" spans="9:24" x14ac:dyDescent="0.35">
       <c r="I32" s="6">
         <v>45</v>
       </c>
@@ -10470,7 +10470,7 @@
         <v>0.26666666666666661</v>
       </c>
     </row>
-    <row r="33" spans="9:16">
+    <row r="33" spans="9:16" x14ac:dyDescent="0.35">
       <c r="I33" s="6">
         <v>50</v>
       </c>
@@ -10486,7 +10486,7 @@
         <v>0.5299999999999998</v>
       </c>
     </row>
-    <row r="34" spans="9:16">
+    <row r="34" spans="9:16" x14ac:dyDescent="0.35">
       <c r="I34" s="6">
         <v>50</v>
       </c>
@@ -10502,7 +10502,7 @@
         <v>0.70100000000000007</v>
       </c>
     </row>
-    <row r="35" spans="9:16">
+    <row r="35" spans="9:16" x14ac:dyDescent="0.35">
       <c r="I35" s="6">
         <v>50</v>
       </c>
@@ -10518,7 +10518,7 @@
         <v>1.5499999999999998</v>
       </c>
     </row>
-    <row r="36" spans="9:16">
+    <row r="36" spans="9:16" x14ac:dyDescent="0.35">
       <c r="I36" s="6">
         <v>50</v>
       </c>
@@ -10534,7 +10534,7 @@
         <v>0.79999999999999982</v>
       </c>
     </row>
-    <row r="37" spans="9:16">
+    <row r="37" spans="9:16" x14ac:dyDescent="0.35">
       <c r="I37" s="6">
         <v>50</v>
       </c>
@@ -10550,22 +10550,22 @@
         <v>0.91999999999999993</v>
       </c>
     </row>
-    <row r="38" spans="9:16">
+    <row r="38" spans="9:16" x14ac:dyDescent="0.35">
       <c r="P38" s="11"/>
     </row>
-    <row r="39" spans="9:16">
+    <row r="39" spans="9:16" x14ac:dyDescent="0.35">
       <c r="P39" s="11"/>
     </row>
-    <row r="40" spans="9:16">
+    <row r="40" spans="9:16" x14ac:dyDescent="0.35">
       <c r="P40" s="11"/>
     </row>
-    <row r="41" spans="9:16">
+    <row r="41" spans="9:16" x14ac:dyDescent="0.35">
       <c r="P41" s="11"/>
     </row>
-    <row r="45" spans="9:16">
+    <row r="45" spans="9:16" x14ac:dyDescent="0.35">
       <c r="O45"/>
     </row>
-    <row r="46" spans="9:16">
+    <row r="46" spans="9:16" x14ac:dyDescent="0.35">
       <c r="O46"/>
     </row>
   </sheetData>
@@ -10583,7 +10583,7 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="9" max="9" width="21" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="5.86328125" bestFit="1" customWidth="1"/>
@@ -10594,7 +10594,7 @@
     <col min="15" max="15" width="7.73046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="13.5" thickBot="1">
+    <row r="1" spans="1:17" ht="13.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>146</v>
       </c>
@@ -10633,7 +10633,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="13.5" thickBot="1">
+    <row r="2" spans="1:17" ht="13.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D2" t="s">
         <v>52</v>
       </c>
@@ -10654,7 +10654,7 @@
       <c r="P2" s="10"/>
       <c r="Q2" s="11"/>
     </row>
-    <row r="3" spans="1:17" ht="13.5" thickBot="1">
+    <row r="3" spans="1:17" ht="13.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="I3" s="17">
         <v>50</v>
       </c>
@@ -10685,7 +10685,7 @@
         <v>1.7167999999999997</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="13.5" thickBot="1">
+    <row r="4" spans="1:17" ht="13.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="I4" s="17">
         <v>45</v>
       </c>
@@ -10716,7 +10716,7 @@
         <v>1.79</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="13.5" thickBot="1">
+    <row r="5" spans="1:17" ht="13.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="I5" s="17">
         <v>45</v>
       </c>
@@ -10747,7 +10747,7 @@
         <v>1.6466666666666669</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="13.5" thickBot="1">
+    <row r="6" spans="1:17" ht="13.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="I6" s="17">
         <v>50</v>
       </c>
@@ -10778,7 +10778,7 @@
         <v>0.99379999999999957</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="13.5" thickBot="1">
+    <row r="7" spans="1:17" ht="13.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="I7" s="17">
         <v>45</v>
       </c>
@@ -10809,7 +10809,7 @@
         <v>1.0926666666666667</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="13.5" thickBot="1">
+    <row r="8" spans="1:17" ht="13.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="I8" s="17">
         <v>50</v>
       </c>
@@ -10840,7 +10840,7 @@
         <v>0.85039999999999982</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="13.5" thickBot="1">
+    <row r="9" spans="1:17" ht="13.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="I9" s="17">
         <v>50</v>
       </c>
@@ -10871,7 +10871,7 @@
         <v>0.73939999999999984</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="13.5" thickBot="1">
+    <row r="10" spans="1:17" ht="13.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="I10" s="17">
         <v>40</v>
       </c>
@@ -10902,7 +10902,7 @@
         <v>1.0632500000000005</v>
       </c>
     </row>
-    <row r="11" spans="1:17" ht="13.5" thickBot="1">
+    <row r="11" spans="1:17" ht="13.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="I11" s="17">
         <v>50</v>
       </c>
@@ -10933,7 +10933,7 @@
         <v>0.59899999999999975</v>
       </c>
     </row>
-    <row r="12" spans="1:17" ht="13.5" thickBot="1">
+    <row r="12" spans="1:17" ht="13.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="I12" s="17">
         <v>35</v>
       </c>
@@ -10964,7 +10964,7 @@
         <v>1.1994285714285713</v>
       </c>
     </row>
-    <row r="13" spans="1:17" ht="13.5" thickBot="1">
+    <row r="13" spans="1:17" ht="13.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="I13" s="17">
         <v>45</v>
       </c>
@@ -10995,7 +10995,7 @@
         <v>0.68599999999999994</v>
       </c>
     </row>
-    <row r="14" spans="1:17" ht="13.5" thickBot="1">
+    <row r="14" spans="1:17" ht="13.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="I14" s="17">
         <v>40</v>
       </c>
@@ -11026,7 +11026,7 @@
         <v>0.81950000000000034</v>
       </c>
     </row>
-    <row r="15" spans="1:17" ht="13.5" thickBot="1">
+    <row r="15" spans="1:17" ht="13.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="I15" s="17">
         <v>50</v>
       </c>
@@ -11057,7 +11057,7 @@
         <v>0.45199999999999996</v>
       </c>
     </row>
-    <row r="16" spans="1:17" ht="13.5" thickBot="1">
+    <row r="16" spans="1:17" ht="13.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="I16" s="17">
         <v>50</v>
       </c>
@@ -11088,7 +11088,7 @@
         <v>0.41119999999999979</v>
       </c>
     </row>
-    <row r="17" spans="9:17" ht="13.5" thickBot="1">
+    <row r="17" spans="9:17" ht="13.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="I17" s="17">
         <v>40</v>
       </c>
@@ -11119,7 +11119,7 @@
         <v>0.59750000000000014</v>
       </c>
     </row>
-    <row r="18" spans="9:17" ht="13.5" thickBot="1">
+    <row r="18" spans="9:17" ht="13.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="I18" s="17">
         <v>35</v>
       </c>
@@ -11150,7 +11150,7 @@
         <v>0.7571428571428569</v>
       </c>
     </row>
-    <row r="19" spans="9:17" ht="13.5" thickBot="1">
+    <row r="19" spans="9:17" ht="13.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="I19" s="17">
         <v>45</v>
       </c>
@@ -11181,7 +11181,7 @@
         <v>0.36133333333333351</v>
       </c>
     </row>
-    <row r="20" spans="9:17" ht="13.5" thickBot="1">
+    <row r="20" spans="9:17" ht="13.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="I20" s="17">
         <v>30</v>
       </c>
@@ -11212,7 +11212,7 @@
         <v>1.0270000000000001</v>
       </c>
     </row>
-    <row r="21" spans="9:17" ht="13.5" thickBot="1">
+    <row r="21" spans="9:17" ht="13.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="I21" s="17">
         <v>30</v>
       </c>
@@ -11243,7 +11243,7 @@
         <v>0.94899999999999984</v>
       </c>
     </row>
-    <row r="22" spans="9:17" ht="13.5" thickBot="1">
+    <row r="22" spans="9:17" ht="13.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="I22" s="17">
         <v>40</v>
       </c>
@@ -11274,7 +11274,7 @@
         <v>0.43625000000000003</v>
       </c>
     </row>
-    <row r="23" spans="9:17" ht="13.5" thickBot="1">
+    <row r="23" spans="9:17" ht="13.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="I23" s="17">
         <v>45</v>
       </c>
@@ -11305,7 +11305,7 @@
         <v>0.2306666666666668</v>
       </c>
     </row>
-    <row r="24" spans="9:17" ht="13.5" thickBot="1">
+    <row r="24" spans="9:17" ht="13.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="I24" s="17">
         <v>40</v>
       </c>
@@ -11336,7 +11336,7 @@
         <v>0.34550000000000014</v>
       </c>
     </row>
-    <row r="25" spans="9:17" ht="13.5" thickBot="1">
+    <row r="25" spans="9:17" ht="13.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="I25" s="17">
         <v>35</v>
       </c>
@@ -11367,7 +11367,7 @@
         <v>0.53342857142857136</v>
       </c>
     </row>
-    <row r="26" spans="9:17" ht="13.5" thickBot="1">
+    <row r="26" spans="9:17" ht="13.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="I26" s="17">
         <v>35</v>
       </c>
@@ -11398,7 +11398,7 @@
         <v>0.48885714285714288</v>
       </c>
     </row>
-    <row r="27" spans="9:17" ht="13.5" thickBot="1">
+    <row r="27" spans="9:17" ht="13.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="I27" s="17">
         <v>30</v>
       </c>
@@ -11429,7 +11429,7 @@
         <v>0.61299999999999999</v>
       </c>
     </row>
-    <row r="28" spans="9:17" ht="13.5" thickBot="1">
+    <row r="28" spans="9:17" ht="13.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="I28" s="17">
         <v>35</v>
       </c>
@@ -11460,7 +11460,7 @@
         <v>0.31742857142857117</v>
       </c>
     </row>
-    <row r="29" spans="9:17" ht="13.5" thickBot="1">
+    <row r="29" spans="9:17" ht="13.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="I29" s="17">
         <v>40</v>
       </c>
@@ -11492,7 +11492,7 @@
         <v>0.11975000000000002</v>
       </c>
     </row>
-    <row r="30" spans="9:17" ht="13.5" thickBot="1">
+    <row r="30" spans="9:17" ht="13.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="I30" s="17">
         <v>30</v>
       </c>
@@ -11523,7 +11523,7 @@
         <v>0.32899999999999996</v>
       </c>
     </row>
-    <row r="31" spans="9:17" ht="13.15">
+    <row r="31" spans="9:17" ht="13.15" x14ac:dyDescent="0.35">
       <c r="I31" s="17">
         <v>35</v>
       </c>
@@ -11571,9 +11571,9 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>156</v>
       </c>
@@ -11582,7 +11582,7 @@
         <v>791.56501207040003</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>157</v>
       </c>
@@ -11593,7 +11593,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>158</v>
       </c>
@@ -11610,12 +11610,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008A7FF1A96F00B548AE8FA4D86E5C3C6B" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="42484d4aadc485b95868b0614c9cc901">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="2de6f903-a70b-4d4e-9d47-d88418a90129" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2e3f4261295b63ab975c65a36ef5f926" ns2:_="">
     <xsd:import namespace="2de6f903-a70b-4d4e-9d47-d88418a90129"/>
@@ -11759,6 +11753,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -11769,22 +11769,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EA26AA80-DA6A-2C4C-8189-C87652E938E8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="2de6f903-a70b-4d4e-9d47-d88418a90129"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F93490E2-E40C-41B2-8038-9CAF72FFFCDE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -11802,6 +11786,22 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EA26AA80-DA6A-2C4C-8189-C87652E938E8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="2de6f903-a70b-4d4e-9d47-d88418a90129"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6736099F-A467-4EDF-97E1-862A5565D775}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Updated model. Has latest task 3 runs and the template for task 4.
</commit_message>
<xml_diff>
--- a/cost_model/cost_model.xlsx
+++ b/cost_model/cost_model.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\knech\OneDrive\Documents\ASE6002\ModelProject\cost_model\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\knech\Documents\ASE6002\ModelProject\cost_model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B419944E-7C9D-4821-9DB0-661A8B92BD60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9973183F-3D45-4324-A8D0-54D49B515783}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="3" xr2:uid="{0BE88EB2-3A1E-BD41-82F4-6438F84B674A}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" activeTab="2" xr2:uid="{0BE88EB2-3A1E-BD41-82F4-6438F84B674A}"/>
   </bookViews>
   <sheets>
     <sheet name="CHAINSAW" sheetId="7" r:id="rId1"/>
@@ -633,9 +633,6 @@
     <t>Compatible Bar Length (cm)</t>
   </si>
   <si>
-    <t>cm</t>
-  </si>
-  <si>
     <t>varCost</t>
   </si>
   <si>
@@ -724,6 +721,9 @@
   </si>
   <si>
     <t>meters</t>
+  </si>
+  <si>
+    <t>m</t>
   </si>
 </sst>
 </file>
@@ -6525,7 +6525,7 @@
       </c>
       <c r="B8" s="32"/>
       <c r="D8" s="28" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="13.15" thickBot="1" x14ac:dyDescent="0.4">
@@ -6542,13 +6542,13 @@
         <v>32</v>
       </c>
       <c r="D10" s="25" t="s">
+        <v>159</v>
+      </c>
+      <c r="G10" s="34" t="s">
         <v>160</v>
       </c>
-      <c r="G10" s="34" t="s">
+      <c r="H10" s="35" t="s">
         <v>161</v>
-      </c>
-      <c r="H10" s="35" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
@@ -6557,10 +6557,10 @@
       </c>
       <c r="B11" s="32"/>
       <c r="D11" s="25" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G11" s="36" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H11" s="37">
         <f>I11*110000</f>
@@ -6576,14 +6576,14 @@
       </c>
       <c r="B12" s="32"/>
       <c r="D12" s="25" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G12" s="39" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="H12" s="32">
         <f>(I36+7000)*12</f>
-        <v>307500</v>
+        <v>262800</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
@@ -6594,10 +6594,10 @@
         <v>13</v>
       </c>
       <c r="D13" s="25" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G13" s="39" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="H13" s="32">
         <f>2*I11*55*2080</f>
@@ -6612,7 +6612,7 @@
         <v>24</v>
       </c>
       <c r="G14" s="40" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H14" s="41">
         <f>(100000+150000+250000)*I14</f>
@@ -6628,17 +6628,17 @@
       </c>
       <c r="B15" s="32"/>
       <c r="D15" s="25" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E15" s="25">
         <v>13</v>
       </c>
       <c r="G15" s="42" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H15" s="43">
         <f>SUM(H11:H14)</f>
-        <v>3199100</v>
+        <v>3154400</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="13.15" thickBot="1" x14ac:dyDescent="0.4">
@@ -6655,10 +6655,10 @@
         <v>15</v>
       </c>
       <c r="G17" s="26" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="H17" s="44" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.35">
@@ -6667,7 +6667,7 @@
       </c>
       <c r="B18" s="32"/>
       <c r="G18" s="45" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H18" s="30">
         <v>8</v>
@@ -6681,14 +6681,14 @@
         <v>30</v>
       </c>
       <c r="C19" s="25" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E19" s="47">
         <f>140*H36</f>
-        <v>3500000</v>
+        <v>2800000</v>
       </c>
       <c r="G19" s="39" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="H19" s="32">
         <v>3</v>
@@ -6700,13 +6700,13 @@
       </c>
       <c r="B20" s="32"/>
       <c r="C20" s="25" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D20" s="25" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="G20" s="39" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="H20" s="48">
         <v>7</v>
@@ -6720,7 +6720,7 @@
         <v>52</v>
       </c>
       <c r="G21" s="39" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H21" s="48">
         <v>11</v>
@@ -6732,7 +6732,7 @@
       </c>
       <c r="B22" s="32"/>
       <c r="G22" s="40" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="H22" s="41">
         <v>4</v>
@@ -6744,7 +6744,7 @@
       </c>
       <c r="B23" s="32"/>
       <c r="G23" s="49" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.35">
@@ -6762,7 +6762,7 @@
       </c>
       <c r="B25" s="32"/>
       <c r="G25" s="51" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.35">
@@ -6771,7 +6771,7 @@
       </c>
       <c r="B26" s="32"/>
       <c r="G26" s="51" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="13.15" thickBot="1" x14ac:dyDescent="0.4">
@@ -6780,7 +6780,7 @@
       </c>
       <c r="B27" s="32"/>
       <c r="G27" s="52" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.35">
@@ -6814,7 +6814,7 @@
         <v>6.4500000000000002E-2</v>
       </c>
       <c r="F31" s="25" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.35">
@@ -6865,11 +6865,11 @@
         <v>0.745</v>
       </c>
       <c r="H36" s="38">
-        <v>25000</v>
+        <v>20000</v>
       </c>
       <c r="I36" s="53">
         <f>G36*H36</f>
-        <v>18625</v>
+        <v>14900</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.35">
@@ -6880,12 +6880,12 @@
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.35">
       <c r="G44" s="25" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.35">
       <c r="G45" s="25" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="H45" s="47">
         <v>1709800</v>
@@ -9625,8 +9625,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:X46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
@@ -9655,14 +9655,14 @@
         <v>0.4</v>
       </c>
       <c r="C2" t="s">
-        <v>155</v>
+        <v>185</v>
       </c>
       <c r="D2" t="s">
         <v>121</v>
       </c>
       <c r="E2" s="10">
-        <f>0.0408*(B2/10)^2-1.7314*(B2/10)+46.597</f>
-        <v>46.52780928</v>
+        <f>0.0408*(B2*100)^2-1.7314*(B2*100)+46.597</f>
+        <v>42.621000000000002</v>
       </c>
       <c r="F2" t="s">
         <v>58</v>
@@ -9691,8 +9691,8 @@
         <v>52</v>
       </c>
       <c r="E3">
-        <f>(B2/10)*0.06</f>
-        <v>2.3999999999999998E-3</v>
+        <f>(B2*100)/55</f>
+        <v>0.72727272727272729</v>
       </c>
       <c r="F3" t="s">
         <v>153</v>
@@ -10579,7 +10579,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD3D1116-BEE9-834A-8EE9-D7FE57E68E2D}">
   <dimension ref="A1:Q31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
@@ -10599,17 +10599,17 @@
         <v>146</v>
       </c>
       <c r="B1">
-        <v>0.4</v>
+        <v>0.33001066910531901</v>
       </c>
       <c r="C1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D1" t="s">
         <v>121</v>
       </c>
       <c r="E1" s="10">
-        <f>-0.0064*(B1/10)^3+0.7895*(B1/10)^2-30.989*(B1/10)+410.5</f>
-        <v>409.26170279040002</v>
+        <f>-0.0064*(B1*100)^3+0.7895*(B1*100)^2-30.989*(B1*100)+410.5</f>
+        <v>17.631923375136012</v>
       </c>
       <c r="I1" s="16" t="s">
         <v>122</v>
@@ -10638,8 +10638,8 @@
         <v>52</v>
       </c>
       <c r="E2">
-        <f>(B1/10)*0.1</f>
-        <v>4.0000000000000001E-3</v>
+        <f>(B1*100)*0.015</f>
+        <v>0.49501600365797854</v>
       </c>
       <c r="F2" t="s">
         <v>153</v>
@@ -11575,33 +11575,33 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B1">
         <f>sawCost+barCost+B3+B4</f>
-        <v>791.56501207040003</v>
+        <v>467.68762216129886</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B3">
-        <v>267.64749999999998</v>
+        <v>339.10668769410398</v>
       </c>
       <c r="C3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B4">
-        <v>68.128</v>
+        <v>68.328011092058901</v>
       </c>
       <c r="C4" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
   </sheetData>
@@ -11610,6 +11610,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008A7FF1A96F00B548AE8FA4D86E5C3C6B" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="42484d4aadc485b95868b0614c9cc901">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="2de6f903-a70b-4d4e-9d47-d88418a90129" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2e3f4261295b63ab975c65a36ef5f926" ns2:_="">
     <xsd:import namespace="2de6f903-a70b-4d4e-9d47-d88418a90129"/>
@@ -11753,12 +11759,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -11769,6 +11769,22 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EA26AA80-DA6A-2C4C-8189-C87652E938E8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="2de6f903-a70b-4d4e-9d47-d88418a90129"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F93490E2-E40C-41B2-8038-9CAF72FFFCDE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -11786,22 +11802,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EA26AA80-DA6A-2C4C-8189-C87652E938E8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="2de6f903-a70b-4d4e-9d47-d88418a90129"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6736099F-A467-4EDF-97E1-862A5565D775}">
   <ds:schemaRefs>

</xml_diff>